<commit_message>
maj2 architecture logicielle et diagramme de sequence
</commit_message>
<xml_diff>
--- a/Block1-Diagramme de séquence.xlsx
+++ b/Block1-Diagramme de séquence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDI-BLOCK1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C7A5D5-BC15-4865-950D-255E6F54D0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C360158-98A3-4E7F-8C20-EFD97A228C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F52B454F-7F36-49AF-84BB-9CF0CF9013E0}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Loop</t>
-  </si>
-  <si>
-    <t>Demande de ticket</t>
   </si>
   <si>
     <t>Base de données</t>
@@ -159,9 +156,6 @@
     <t>Demander paiement en ligne</t>
   </si>
   <si>
-    <t>[tant que paiement non valide]</t>
-  </si>
-  <si>
     <t>Envoi informations paiement</t>
   </si>
   <si>
@@ -177,10 +171,20 @@
     <t>Paiement non valide</t>
   </si>
   <si>
-    <t>Enregistrement eventuel infos paiement</t>
+    <t>[Choix de l'utilisateur de conserver les infos de paiement]]</t>
   </si>
   <si>
-    <t>Confirmation enregistrement infos paiement</t>
+    <t>Enregistrement infos paiement</t>
+  </si>
+  <si>
+    <t>Confirmation enregistrement infos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demande de ticket
+(nb tickets, conservation infos paiement o/n) </t>
+  </si>
+  <si>
+    <t>[paiement non valide ou délai dépassé]</t>
   </si>
 </sst>
 </file>
@@ -204,7 +208,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="22"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -237,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -260,16 +264,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -297,10 +304,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>714375</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -345,7 +352,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>894522</xdr:colOff>
+      <xdr:colOff>1581150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -368,8 +375,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5085522" y="0"/>
-          <a:ext cx="1500394" cy="779807"/>
+          <a:off x="5648325" y="0"/>
+          <a:ext cx="1504950" cy="666749"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -414,7 +421,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>616324</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -470,7 +477,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>403412</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -524,15 +531,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>428625</xdr:rowOff>
+      <xdr:rowOff>628650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>428625</xdr:rowOff>
+      <xdr:rowOff>628650</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -547,8 +554,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3400425" y="1971675"/>
-          <a:ext cx="1752600" cy="0"/>
+          <a:off x="3800475" y="1171575"/>
+          <a:ext cx="2362200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -955,7 +962,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>11206</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -970,8 +977,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="760320" y="2151529"/>
-          <a:ext cx="9414621" cy="3361764"/>
+          <a:off x="762001" y="2219325"/>
+          <a:ext cx="11117355" cy="4324350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1643,13 +1650,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1696,7 +1703,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>733632</xdr:colOff>
+      <xdr:colOff>733425</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
@@ -1721,8 +1728,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5835719" y="779807"/>
-          <a:ext cx="9318" cy="288000"/>
+          <a:off x="6400800" y="666749"/>
+          <a:ext cx="9525" cy="288000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1758,7 +1765,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>770282</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>248478</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1806,15 +1813,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>750795</xdr:colOff>
+      <xdr:colOff>752475</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>616324</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1827,12 +1834,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
+          <a:endCxn id="97" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9760324" y="12550588"/>
-          <a:ext cx="11205" cy="1400736"/>
+          <a:off x="11087100" y="12639675"/>
+          <a:ext cx="9525" cy="4000499"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2703,13 +2711,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>717176</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>403412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>627529</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3441,7 +3449,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>140804</xdr:rowOff>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3456,13 +3464,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8283" y="14718196"/>
-          <a:ext cx="14386891" cy="2335695"/>
+          <a:off x="8283" y="13001625"/>
+          <a:ext cx="13926792" cy="2695575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln w="25400"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3555,22 +3564,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>60882</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>5798</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>80762</xdr:rowOff>
+      <xdr:colOff>28155</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>3330</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>26913</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>346232</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle : avec coin rogné 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9E563BF-8A1B-4ED3-B410-E64663AE40B0}"/>
+        <xdr:cNvPr id="18" name="Rectangle : avec coin rogné 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{271DC03A-9840-4293-85F1-5503CB6306BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3578,7 +3587,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="957262" y="5976943"/>
+          <a:off x="232942" y="14715521"/>
           <a:ext cx="342902" cy="752475"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -3617,39 +3626,92 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>28155</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>3330</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>26913</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>346232</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>216833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>216833</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connecteur droit avec flèche 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC0CC7D-1A02-4080-A4F2-8E5796F8564A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3790950" y="9369116"/>
+          <a:ext cx="1901687" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="lgDash"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Rectangle : avec coin rogné 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{271DC03A-9840-4293-85F1-5503CB6306BE}"/>
+        <xdr:cNvPr id="32" name="Rectangle 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9DCC0AF-CBBF-486D-827C-5CA3AB0F0CCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="232942" y="14715521"/>
-          <a:ext cx="342902" cy="752475"/>
-        </a:xfrm>
-        <a:prstGeom prst="snip1Rect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 35535"/>
-          </a:avLst>
+        <a:xfrm>
+          <a:off x="9925049" y="9524"/>
+          <a:ext cx="1409287" cy="789333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln w="25400"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3680,23 +3742,81 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>216833</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>216833</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>690866</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>753717</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>256761</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Connecteur droit avec flèche 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC0CC7D-1A02-4080-A4F2-8E5796F8564A}"/>
+        <xdr:cNvPr id="35" name="Connecteur droit 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5D48ACA-993E-4E7D-A54C-1D9E3016B075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12758627" y="782730"/>
+          <a:ext cx="62851" cy="14192227"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="lgDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>853109</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>405847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>588065</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>414131</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Connecteur droit avec flèche 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB8D0F0D-B99E-45D1-8A8D-4F2F5829A538}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3704,15 +3824,15 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3790950" y="9369116"/>
-          <a:ext cx="1901687" cy="0"/>
+          <a:off x="5955196" y="15513325"/>
+          <a:ext cx="6700630" cy="8284"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
-          <a:prstDash val="lgDash"/>
-          <a:tailEnd type="arrow"/>
+          <a:prstDash val="solid"/>
+          <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -3735,22 +3855,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:colOff>591476</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>283558</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>877226</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>496956</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="Rectangle 31">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9DCC0AF-CBBF-486D-827C-5CA3AB0F0CCD}"/>
+        <xdr:cNvPr id="41" name="Rectangle 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7503DA95-FD4A-4A67-B669-71F18572F994}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3758,14 +3878,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9925049" y="9524"/>
-          <a:ext cx="1409287" cy="789333"/>
+          <a:off x="13081650" y="15001754"/>
+          <a:ext cx="285750" cy="1985876"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln w="25400"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3796,179 +3915,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>690866</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12447</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>753717</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>256761</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="35" name="Connecteur droit 34">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5D48ACA-993E-4E7D-A54C-1D9E3016B075}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12758627" y="782730"/>
-          <a:ext cx="62851" cy="14192227"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:prstDash val="lgDash"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>853109</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>405847</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>588065</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>414131</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="39" name="Connecteur droit avec flèche 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB8D0F0D-B99E-45D1-8A8D-4F2F5829A538}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5955196" y="15513325"/>
-          <a:ext cx="6700630" cy="8284"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="solid"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>591476</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>283558</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>877226</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>496956</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="Rectangle 40">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7503DA95-FD4A-4A67-B669-71F18572F994}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13081650" y="15001754"/>
-          <a:ext cx="285750" cy="1985876"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>8282</xdr:colOff>
       <xdr:row>35</xdr:row>
@@ -4000,6 +3946,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln w="25400"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -4368,14 +4315,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>621196</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>248480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>906946</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>389283</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4390,8 +4337,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8779566" y="17161567"/>
-          <a:ext cx="285750" cy="728868"/>
+          <a:off x="8784121" y="15717080"/>
+          <a:ext cx="285750" cy="675445"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4429,13 +4376,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>891623</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>419100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>596348</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>428625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4482,13 +4429,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>882098</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>249038</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>586823</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>249038</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4589,15 +4536,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>768724</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>389283</xdr:rowOff>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>786847</xdr:colOff>
+      <xdr:colOff>790575</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>563217</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4608,12 +4555,14 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="98" idx="0"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8927094" y="18370826"/>
-          <a:ext cx="18123" cy="612913"/>
+          <a:off x="8934450" y="16421100"/>
+          <a:ext cx="19050" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4649,7 +4598,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>737152</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>546652</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4698,13 +4647,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4751,13 +4700,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>885825</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>276225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4805,13 +4754,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>5</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>342907</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4868,13 +4817,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>390524</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4928,15 +4877,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>414618</xdr:rowOff>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4951,8 +4900,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8729870" y="13401261"/>
-          <a:ext cx="285750" cy="803900"/>
+          <a:off x="8810625" y="17373600"/>
+          <a:ext cx="285750" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4990,13 +4939,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>425825</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>493059</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5052,14 +5001,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5074,8 +5023,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6144039" y="13610811"/>
-          <a:ext cx="2595356" cy="9525"/>
+          <a:off x="6143625" y="17583150"/>
+          <a:ext cx="2676525" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5105,14 +5054,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>235883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>235883</xdr:rowOff>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5126,9 +5075,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6124989" y="14026426"/>
-          <a:ext cx="2595356" cy="0"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6124575" y="18047633"/>
+          <a:ext cx="2686050" cy="2242"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5153,6 +5102,237 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>609600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Connecteur droit 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FE41362-807F-4B37-A15E-864C2C0173E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8972550" y="18116550"/>
+          <a:ext cx="0" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="lgDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>571500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Connecteur droit 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{951F7584-9142-49A8-B1B6-095EAC11F22F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11058525" y="17316450"/>
+          <a:ext cx="9525" cy="1504950"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="lgDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>504824</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Rectangle 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5A7D065-EF8A-D765-8715-93708D8712B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4191000" y="15859124"/>
+          <a:ext cx="5248275" cy="1438275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>11596</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>3319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>764071</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>346221</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Rectangle : avec coin rogné 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{544D3E24-544B-4D51-87D7-CEDF203E9CE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4407383" y="16105332"/>
+          <a:ext cx="342902" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 35535"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5455,10 +5635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D53F07A-3961-40C4-86DD-74C26093B63D}">
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5467,43 +5647,44 @@
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="21.140625" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
     <col min="13" max="13" width="17.140625" customWidth="1"/>
     <col min="14" max="14" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
-        <v>24</v>
+    <row r="1" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="G1" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="1" t="s">
-        <v>1</v>
+    <row r="2" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5512,16 +5693,16 @@
     </row>
     <row r="4" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="F4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -5533,12 +5714,12 @@
     <row r="6" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="F6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5546,7 +5727,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="F7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5554,29 +5735,29 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="F8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3"/>
       <c r="F9" s="6"/>
       <c r="J9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10" s="6"/>
       <c r="J10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5584,7 +5765,7 @@
       <c r="D11" s="3"/>
       <c r="F11" s="6"/>
       <c r="H11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5593,17 +5774,17 @@
       <c r="D12" s="3"/>
       <c r="F12" s="6"/>
       <c r="H12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -5612,14 +5793,14 @@
     <row r="15" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="3"/>
       <c r="F15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -5646,11 +5827,11 @@
     <row r="20" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5659,14 +5840,14 @@
       <c r="C21" s="5"/>
       <c r="F21" s="4"/>
       <c r="H21" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -5674,10 +5855,10 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5685,7 +5866,7 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="F24" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24" s="6"/>
     </row>
@@ -5694,7 +5875,7 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="F25" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H25" s="6"/>
     </row>
@@ -5703,7 +5884,7 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -5712,10 +5893,10 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H27" s="6"/>
     </row>
@@ -5724,31 +5905,31 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="E29" s="1"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5772,7 +5953,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="F33" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H33" s="6"/>
     </row>
@@ -5786,24 +5967,24 @@
     </row>
     <row r="35" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="10" t="s">
-        <v>4</v>
+      <c r="D36" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="H36" s="2"/>
     </row>
@@ -5811,121 +5992,129 @@
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="11" t="s">
-        <v>44</v>
+      <c r="D37" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="H37" s="2"/>
       <c r="J37" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="10" t="s">
-        <v>35</v>
+      <c r="D38" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H38" s="2"/>
       <c r="J38" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="8"/>
+      <c r="F39" s="1"/>
+      <c r="H39" s="2"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H40" s="2"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="F41" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="F39" s="1"/>
-      <c r="H39" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="F40" s="1"/>
-      <c r="H40" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="F41" s="1"/>
-      <c r="J41" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="42" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="F42" s="1"/>
-      <c r="J42" s="2" t="s">
-        <v>21</v>
+      <c r="H42" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="A43" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="F43" s="4"/>
-      <c r="H43" s="6" t="s">
-        <v>16</v>
+      <c r="F43" s="1"/>
+      <c r="J43" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="A44" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="1"/>
-      <c r="H44" s="6" t="s">
-        <v>38</v>
+      <c r="J44" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
-      <c r="F45" s="6" t="s">
-        <v>22</v>
+      <c r="F45" s="4"/>
+      <c r="H45" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
+      <c r="F46" s="1"/>
+      <c r="H46" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="47" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="F47" s="1"/>
+      <c r="F47" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="48" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
@@ -5933,7 +6122,6 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="F49" s="1"/>
-      <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
@@ -5941,7 +6129,6 @@
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="F50" s="1"/>
-      <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -5949,6 +6136,7 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="F51" s="1"/>
+      <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
@@ -5956,6 +6144,7 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="F52" s="1"/>
+      <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
@@ -5971,15 +6160,27 @@
       <c r="D54" s="3"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
+      <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6002,12 +6203,14 @@
     <row r="78" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="1.1023622047244095" right="0.31496062992125984" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="48" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="39" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
maj3 architecture logicielle et diagramme de sequence
</commit_message>
<xml_diff>
--- a/Block1-Diagramme de séquence.xlsx
+++ b/Block1-Diagramme de séquence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDI-BLOCK1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C360158-98A3-4E7F-8C20-EFD97A228C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BB7E73-D14D-4FC7-8305-1B77BB3EE6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F52B454F-7F36-49AF-84BB-9CF0CF9013E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Loop</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Demander paiement en ligne</t>
   </si>
   <si>
-    <t>Envoi informations paiement</t>
-  </si>
-  <si>
     <t>Paiement en ligne</t>
   </si>
   <si>
@@ -171,20 +168,27 @@
     <t>Paiement non valide</t>
   </si>
   <si>
-    <t>[Choix de l'utilisateur de conserver les infos de paiement]]</t>
-  </si>
-  <si>
     <t>Enregistrement infos paiement</t>
   </si>
   <si>
     <t>Confirmation enregistrement infos</t>
   </si>
   <si>
-    <t xml:space="preserve">Demande de ticket
-(nb tickets, conservation infos paiement o/n) </t>
+    <t>[paiement non valide ou délai dépassé]</t>
   </si>
   <si>
-    <t>[paiement non valide ou délai dépassé]</t>
+    <t>Envoi infos paiement
+et choix conservation
+infos paiement</t>
+  </si>
+  <si>
+    <t>Envoi infos paiement</t>
+  </si>
+  <si>
+    <t>[conserver infos paiement]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demande de ticket </t>
   </si>
 </sst>
 </file>
@@ -421,7 +425,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>616324</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -472,12 +476,12 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>285751</xdr:rowOff>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>403412</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -493,8 +497,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5388349" y="1058957"/>
-          <a:ext cx="285750" cy="12679455"/>
+          <a:off x="6143625" y="742950"/>
+          <a:ext cx="285750" cy="18310412"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -531,15 +535,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>628650</xdr:rowOff>
+      <xdr:rowOff>266700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>628650</xdr:rowOff>
+      <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -554,7 +558,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3800475" y="1171575"/>
+          <a:off x="3781425" y="809625"/>
           <a:ext cx="2362200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1650,13 +1654,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1703,7 +1707,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:colOff>742950</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
@@ -1711,7 +1715,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>297524</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1728,8 +1732,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6400800" y="666749"/>
-          <a:ext cx="9525" cy="288000"/>
+          <a:off x="6305550" y="552449"/>
+          <a:ext cx="0" cy="180976"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1764,9 +1768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>770282</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>248478</xdr:rowOff>
+      <xdr:colOff>764071</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1779,12 +1783,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
+          <a:endCxn id="78" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8641197" y="14227573"/>
-          <a:ext cx="30694" cy="2933992"/>
+          <a:off x="9035863" y="10239375"/>
+          <a:ext cx="24483" cy="3886201"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1820,7 +1825,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2604,13 +2609,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>401731</xdr:rowOff>
+      <xdr:rowOff>239806</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>401731</xdr:rowOff>
+      <xdr:rowOff>239806</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2625,8 +2630,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3379694" y="9478496"/>
-          <a:ext cx="1733550" cy="0"/>
+          <a:off x="3771900" y="8393206"/>
+          <a:ext cx="2343150" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2658,13 +2663,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>394448</xdr:rowOff>
+      <xdr:rowOff>251573</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>394448</xdr:rowOff>
+      <xdr:rowOff>251573</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2679,8 +2684,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3379694" y="10053919"/>
-          <a:ext cx="1752600" cy="0"/>
+          <a:off x="3771900" y="8795498"/>
+          <a:ext cx="2362200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2711,13 +2716,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>717176</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>403412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>627529</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2735,7 +2740,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5524500" y="13738412"/>
+          <a:off x="6279776" y="19053362"/>
           <a:ext cx="6724" cy="224117"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2892,13 +2897,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>269501</xdr:rowOff>
+      <xdr:rowOff>212351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>269501</xdr:rowOff>
+      <xdr:rowOff>212351</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2913,8 +2918,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3626224" y="5749177"/>
-          <a:ext cx="1733550" cy="0"/>
+          <a:off x="3771900" y="4508126"/>
+          <a:ext cx="2343150" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2946,13 +2951,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>349622</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>265023</xdr:rowOff>
+      <xdr:rowOff>226923</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>559172</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>265023</xdr:rowOff>
+      <xdr:rowOff>226923</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2967,8 +2972,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3632946" y="6394641"/>
-          <a:ext cx="1733550" cy="0"/>
+          <a:off x="3778622" y="5017998"/>
+          <a:ext cx="2343150" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3000,13 +3005,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>322834</xdr:rowOff>
+      <xdr:rowOff>227584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3021,8 +3026,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5664574" y="4043187"/>
-          <a:ext cx="1752039" cy="10541"/>
+          <a:off x="6419850" y="3951859"/>
+          <a:ext cx="2457450" cy="1016"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3053,13 +3058,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3074,8 +3079,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5664574" y="4426884"/>
-          <a:ext cx="1732989" cy="0"/>
+          <a:off x="6419850" y="4229100"/>
+          <a:ext cx="2438400" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3282,13 +3287,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>349624</xdr:rowOff>
+      <xdr:rowOff>235324</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>359149</xdr:rowOff>
+      <xdr:rowOff>244849</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3303,8 +3308,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5481918" y="5504330"/>
-          <a:ext cx="3916456" cy="9525"/>
+          <a:off x="6438900" y="3283324"/>
+          <a:ext cx="4619625" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3335,13 +3340,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>885825</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>332255</xdr:rowOff>
+      <xdr:rowOff>227480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>351305</xdr:rowOff>
+      <xdr:rowOff>246530</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3356,8 +3361,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="5491443" y="5957608"/>
-          <a:ext cx="3906931" cy="19050"/>
+          <a:off x="6448425" y="3666005"/>
+          <a:ext cx="4610100" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3448,7 +3453,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3511,7 +3516,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>8281</xdr:rowOff>
+      <xdr:rowOff>55906</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3629,13 +3634,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>216833</xdr:rowOff>
+      <xdr:rowOff>578783</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>216833</xdr:rowOff>
+      <xdr:rowOff>578783</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3650,8 +3655,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3790950" y="9369116"/>
-          <a:ext cx="1901687" cy="0"/>
+          <a:off x="3790950" y="13256558"/>
+          <a:ext cx="2362200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3802,14 +3807,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>853109</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>405847</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>215347</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>588065</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>414131</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>223631</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3824,8 +3829,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5955196" y="15513325"/>
-          <a:ext cx="6700630" cy="8284"/>
+          <a:off x="6415709" y="13521772"/>
+          <a:ext cx="6802506" cy="8284"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3862,7 +3867,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>877226</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>496956</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3917,13 +3922,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>8282</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1358348</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3983,13 +3988,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>11596</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>3319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>764071</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>346221</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4045,31 +4050,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>180561</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>190086</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>647286</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>209136</xdr:rowOff>
+      <xdr:colOff>877958</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>207067</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>579783</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>215349</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="61" name="Connecteur droit avec flèche 60">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AF25AC7-CAAD-4153-B403-C7D4604DE2F6}"/>
+        <xdr:cNvPr id="63" name="Connecteur droit avec flèche 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDEB1BFA-4935-414B-8E91-162339B705C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5448300" y="4695825"/>
-          <a:ext cx="4508638" cy="19050"/>
+        <a:xfrm flipH="1">
+          <a:off x="6145697" y="16275328"/>
+          <a:ext cx="6667499" cy="8282"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4098,32 +4103,85 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>332961</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19464</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>37686</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38514</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>770278</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>414130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1335256</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="62" name="Connecteur droit avec flèche 61">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AAB04A8-FC0E-4A3C-AC63-6892D168A013}"/>
+        <xdr:cNvPr id="65" name="Connecteur droit 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CA88E37-3363-490C-9CCA-507C2722C13E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5600700" y="4848225"/>
-          <a:ext cx="4508638" cy="19050"/>
+        <a:xfrm flipV="1">
+          <a:off x="2269430" y="16482391"/>
+          <a:ext cx="11556000" cy="16566"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="lgDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>869673</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>256761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571498</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>265043</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Connecteur droit avec flèche 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{214A2D31-9DA0-42EC-96AA-E916AFA37F67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6137412" y="16747435"/>
+          <a:ext cx="6667499" cy="8282"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4152,177 +4210,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>877958</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>207067</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>579783</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>215349</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="63" name="Connecteur droit avec flèche 62">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDEB1BFA-4935-414B-8E91-162339B705C7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6145697" y="16275328"/>
-          <a:ext cx="6667499" cy="8282"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="lgDash"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>770278</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>414130</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1335256</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>8283</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="65" name="Connecteur droit 64">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CA88E37-3363-490C-9CCA-507C2722C13E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2269430" y="16482391"/>
-          <a:ext cx="11556000" cy="16566"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="lgDash"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>869673</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>256761</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>571498</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>265043</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="Connecteur droit avec flèche 72">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{214A2D31-9DA0-42EC-96AA-E916AFA37F67}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6137412" y="16747435"/>
-          <a:ext cx="6667499" cy="8282"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="lgDash"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>621196</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>248480</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>906946</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>333375</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>333376</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4337,8 +4234,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8784121" y="15717080"/>
-          <a:ext cx="285750" cy="675445"/>
+          <a:off x="8917471" y="14125576"/>
+          <a:ext cx="285750" cy="819150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4376,14 +4273,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>891623</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>596348</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>428625</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4398,8 +4295,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6159362" y="17332187"/>
-          <a:ext cx="2338595" cy="9525"/>
+          <a:off x="6454223" y="14258925"/>
+          <a:ext cx="2438400" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4429,13 +4326,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>882098</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>249038</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>586823</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>249038</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4483,13 +4380,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>356136</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>480394</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>584736</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>480394</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4537,13 +4434,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>771525</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>361950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>790575</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4592,13 +4489,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>734351</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>496956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>737152</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>546652</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4647,14 +4544,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4669,8 +4566,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6144039" y="12927496"/>
-          <a:ext cx="4774924" cy="9525"/>
+          <a:off x="6438900" y="15335250"/>
+          <a:ext cx="4619625" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4700,14 +4597,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>885825</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>276225</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4722,8 +4619,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6153564" y="13288203"/>
-          <a:ext cx="4765399" cy="19050"/>
+          <a:off x="6448425" y="15678150"/>
+          <a:ext cx="4610100" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4754,13 +4651,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>5</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>342907</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4817,13 +4714,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>390524</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4878,13 +4775,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>323850</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4939,13 +4836,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>425825</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>493059</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5001,13 +4898,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5054,13 +4951,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>235883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5108,13 +5005,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>609600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5161,13 +5058,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>381000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>571500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5214,13 +5111,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>504824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5276,13 +5173,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>11596</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>3319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>764071</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>346221</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5635,10 +5532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D53F07A-3961-40C4-86DD-74C26093B63D}">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5674,12 +5571,12 @@
         <v>10</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F2" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5738,49 +5635,49 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="3"/>
       <c r="F9" s="6"/>
-      <c r="J9" s="2" t="s">
+      <c r="I9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10" s="6"/>
-      <c r="J10" s="2" t="s">
+      <c r="I10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="D11" s="3"/>
       <c r="F11" s="6"/>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="6"/>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5790,13 +5687,13 @@
       <c r="D14" s="3"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="C15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5824,7 +5721,7 @@
       <c r="C19" s="3"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>9</v>
@@ -5834,7 +5731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="5"/>
@@ -5843,7 +5740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
@@ -5851,7 +5748,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
@@ -5861,7 +5758,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5870,7 +5767,7 @@
       </c>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5879,7 +5776,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5888,26 +5785,26 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="6" t="s">
         <v>18</v>
       </c>
       <c r="H28" s="6"/>
@@ -5957,7 +5854,7 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5965,163 +5862,163 @@
       <c r="F34" s="1"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="F35" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>39</v>
+      <c r="F35" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="8" t="s">
-        <v>3</v>
+      <c r="D36" s="3"/>
+      <c r="F36" s="10"/>
+      <c r="H36" s="6" t="s">
+        <v>47</v>
       </c>
-      <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="9" t="s">
-        <v>42</v>
+      <c r="D37" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="H37" s="2"/>
-      <c r="J37" s="4" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="38" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>43</v>
+      <c r="D38" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="H38" s="2"/>
       <c r="J38" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="8"/>
-      <c r="F39" s="1"/>
+      <c r="D39" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="H39" s="2"/>
-      <c r="J39" s="4"/>
+      <c r="J39" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="40" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="8"/>
-      <c r="F40" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="F40" s="1"/>
       <c r="H40" s="2"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="D41" s="8"/>
       <c r="F41" s="8" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="H41" s="2"/>
+      <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="F42" s="1"/>
+      <c r="F42" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="H42" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>0</v>
-      </c>
+    <row r="43" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="F43" s="1"/>
-      <c r="J43" s="2" t="s">
-        <v>19</v>
+      <c r="H43" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="1"/>
-      <c r="J44" s="2" t="s">
+      <c r="H44" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="F45" s="1"/>
+      <c r="H45" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="F45" s="4"/>
-      <c r="H45" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="4"/>
       <c r="H46" s="6" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="F47" s="6" t="s">
-        <v>21</v>
+      <c r="F47" s="1"/>
+      <c r="H47" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
+      <c r="F48" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="49" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
@@ -6136,7 +6033,6 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="F51" s="1"/>
-      <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
@@ -6152,6 +6048,7 @@
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="F53" s="1"/>
+      <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
@@ -6174,14 +6071,20 @@
       <c r="D56" s="3"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
+      <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6205,12 +6108,13 @@
     <row r="80" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="60.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="1.1023622047244095" right="0.31496062992125984" top="0.15748031496062992" bottom="0.15748031496062992" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="39" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="43" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>